<commit_message>
PC: Tesis - Listo con la Regresión Logistica
</commit_message>
<xml_diff>
--- a/bdd/dataframe.xlsx
+++ b/bdd/dataframe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abraham\Documents\Machine-Learning-con-Jupiter\bdd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Machine-Learning-con-Jupiter\bdd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89E23B4-C0F3-47E8-8299-AE895F4F171F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A460D1-7E4B-4953-8045-A18E9CC4064F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19140" yWindow="2340" windowWidth="19095" windowHeight="18090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21015" yWindow="0" windowWidth="17385" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="338">
   <si>
     <t>CLAVE</t>
   </si>
@@ -220,9 +220,6 @@
     </r>
   </si>
   <si>
-    <t>NIHSS 6M</t>
-  </si>
-  <si>
     <t>RANKIN 6M</t>
   </si>
   <si>
@@ -622,9 +619,6 @@
     <t>24/07/15</t>
   </si>
   <si>
-    <t>Fallecido???</t>
-  </si>
-  <si>
     <t>acv mayor acm , secuela grave , acudio a control si fallecio fue despues</t>
   </si>
   <si>
@@ -809,9 +803,6 @@
   </si>
   <si>
     <t>ACCIDENTE CEREBROVASCULAR ISQUEMICO</t>
-  </si>
-  <si>
-    <t>Fallecido ???</t>
   </si>
   <si>
     <t>Falla multiorganica</t>
@@ -1104,6 +1095,9 @@
   </si>
   <si>
     <t>Fosfatasa Alcalina</t>
+  </si>
+  <si>
+    <t>NIHSS 6M</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1246,6 +1240,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -1527,10 +1522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CG45"/>
+  <dimension ref="A1:CK45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,9 +1582,11 @@
     <col min="64" max="64" width="13.85546875" customWidth="1"/>
     <col min="65" max="65" width="49.28515625" customWidth="1"/>
     <col min="66" max="85" width="12.42578125" customWidth="1"/>
+    <col min="86" max="86" width="20" customWidth="1"/>
+    <col min="87" max="87" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1681,7 +1678,7 @@
         <v>29</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>30</v>
@@ -1705,7 +1702,7 @@
         <v>36</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="AN1" s="1" t="s">
         <v>37</v>
@@ -1735,10 +1732,10 @@
         <v>45</v>
       </c>
       <c r="AW1" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="AY1" s="2" t="s">
         <v>46</v>
@@ -1747,111 +1744,115 @@
         <v>47</v>
       </c>
       <c r="BA1" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="BB1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="BB1" s="3" t="s">
+      <c r="BC1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BD1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="BD1" s="5" t="s">
+      <c r="BE1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="BE1" s="5" t="s">
+      <c r="BF1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="BF1" s="5" t="s">
+      <c r="BG1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BW1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BV1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CB1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="CB1" s="5" t="s">
+      <c r="CC1" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="CC1" s="6" t="s">
+      <c r="CD1" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="CD1" s="6" t="s">
+      <c r="CE1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="CE1" s="5" t="s">
+      <c r="CF1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="CG1" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="CH1" s="21"/>
+      <c r="CI1" s="21"/>
+      <c r="CJ1" s="21"/>
+      <c r="CK1" s="21"/>
     </row>
-    <row r="2" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:89" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2">
         <v>2012418042</v>
@@ -1951,7 +1952,7 @@
         <v>25.51</v>
       </c>
       <c r="AQ2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AV2" s="7">
         <v>11</v>
@@ -1969,37 +1970,37 @@
         <v>6</v>
       </c>
       <c r="BA2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BB2">
         <v>6</v>
       </c>
       <c r="BC2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="BD2" t="s">
         <v>83</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>84</v>
       </c>
       <c r="BG2" s="8">
         <v>42313</v>
       </c>
       <c r="BH2" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="BI2" s="10">
         <v>42135</v>
       </c>
       <c r="BJ2" t="s">
+        <v>85</v>
+      </c>
+      <c r="BM2" t="s">
         <v>86</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="BN2" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="BN2" s="11" t="s">
+      <c r="BO2" t="s">
         <v>88</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>89</v>
       </c>
       <c r="BR2" s="12">
         <v>54.631620258629141</v>
@@ -2057,16 +2058,20 @@
         <f t="shared" ref="CG2:CG38" si="6">(CE2/BY2)</f>
         <v>-0.82573229757189326</v>
       </c>
+      <c r="CH2" s="21"/>
+      <c r="CI2" s="21"/>
+      <c r="CJ2" s="21"/>
+      <c r="CK2" s="21"/>
     </row>
-    <row r="3" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
         <v>90</v>
-      </c>
-      <c r="C3" t="s">
-        <v>91</v>
       </c>
       <c r="D3">
         <v>2000149601</v>
@@ -2085,16 +2090,16 @@
         <v>165</v>
       </c>
       <c r="I3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" t="s">
         <v>92</v>
       </c>
-      <c r="J3" t="s">
-        <v>92</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>93</v>
-      </c>
-      <c r="L3" t="s">
-        <v>94</v>
       </c>
       <c r="M3">
         <v>56</v>
@@ -2159,7 +2164,7 @@
       <c r="AO3" s="7"/>
       <c r="AP3" s="7"/>
       <c r="AQ3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AV3" s="7">
         <v>15</v>
@@ -2183,22 +2188,22 @@
         <v>2</v>
       </c>
       <c r="BC3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="BD3" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="BD3" s="15" t="s">
+      <c r="BE3" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="BE3" s="15" t="s">
+      <c r="BF3" s="15" t="s">
         <v>98</v>
-      </c>
-      <c r="BF3" s="15" t="s">
-        <v>99</v>
       </c>
       <c r="BG3" s="8">
         <v>42343</v>
       </c>
       <c r="BH3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BR3" s="12">
         <v>118.18672541999449</v>
@@ -2256,16 +2261,20 @@
         <f t="shared" si="6"/>
         <v>-1.081411324865972</v>
       </c>
+      <c r="CH3" s="21"/>
+      <c r="CI3" s="21"/>
+      <c r="CJ3" s="21"/>
+      <c r="CK3" s="21"/>
     </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
         <v>101</v>
-      </c>
-      <c r="C4" t="s">
-        <v>102</v>
       </c>
       <c r="D4">
         <v>98085992</v>
@@ -2278,13 +2287,13 @@
         <v>78</v>
       </c>
       <c r="I4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M4">
         <v>91</v>
@@ -2377,7 +2386,7 @@
         <v>23.4</v>
       </c>
       <c r="AQ4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AV4" s="7">
         <v>15</v>
@@ -2397,22 +2406,22 @@
       <c r="BA4" s="7"/>
       <c r="BB4" s="7"/>
       <c r="BC4" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BD4" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="BE4" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="BE4" s="15" t="s">
+      <c r="BF4" s="15" t="s">
         <v>106</v>
-      </c>
-      <c r="BF4" s="15" t="s">
-        <v>107</v>
       </c>
       <c r="BG4" s="8">
         <v>42343</v>
       </c>
       <c r="BH4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BP4" s="17">
         <v>32500000000</v>
@@ -2476,16 +2485,20 @@
         <f t="shared" si="6"/>
         <v>-0.29681746818343702</v>
       </c>
+      <c r="CH4" s="21"/>
+      <c r="CI4" s="21"/>
+      <c r="CJ4" s="21"/>
+      <c r="CK4" s="21"/>
     </row>
-    <row r="5" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D5">
         <v>9772094</v>
@@ -2501,13 +2514,13 @@
         <v>52.5</v>
       </c>
       <c r="I5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M5">
         <v>59</v>
@@ -2600,7 +2613,7 @@
         <v>22.93</v>
       </c>
       <c r="AQ5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AV5" s="7">
         <v>15</v>
@@ -2624,22 +2637,22 @@
         <v>2</v>
       </c>
       <c r="BC5" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BD5" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="BE5" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="BE5" s="15" t="s">
+      <c r="BF5" s="15" t="s">
         <v>112</v>
-      </c>
-      <c r="BF5" s="15" t="s">
-        <v>113</v>
       </c>
       <c r="BG5" s="8">
         <v>42137</v>
       </c>
       <c r="BH5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BR5" s="12">
         <v>188.90666272666715</v>
@@ -2697,16 +2710,20 @@
         <f t="shared" si="6"/>
         <v>-1.7619964936453375E-2</v>
       </c>
+      <c r="CH5" s="21"/>
+      <c r="CI5" s="21"/>
+      <c r="CJ5" s="21"/>
+      <c r="CK5" s="21"/>
     </row>
-    <row r="6" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" t="s">
         <v>114</v>
-      </c>
-      <c r="C6" t="s">
-        <v>115</v>
       </c>
       <c r="D6">
         <v>98095110</v>
@@ -2722,13 +2739,13 @@
         <v>94</v>
       </c>
       <c r="I6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M6">
         <v>104</v>
@@ -2809,7 +2826,7 @@
         <v>103.8</v>
       </c>
       <c r="AQ6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AV6" s="7">
         <v>15</v>
@@ -2833,29 +2850,29 @@
         <v>1</v>
       </c>
       <c r="BC6" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD6" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="BE6" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="BE6" s="15" t="s">
-        <v>118</v>
-      </c>
       <c r="BF6" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BG6" s="8"/>
       <c r="BH6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM6" t="s">
+        <v>118</v>
+      </c>
+      <c r="BN6" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO6" t="s">
         <v>119</v>
-      </c>
-      <c r="BN6" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="BO6" t="s">
-        <v>120</v>
       </c>
       <c r="BP6" s="17">
         <v>248000000</v>
@@ -2919,16 +2936,20 @@
         <f t="shared" si="6"/>
         <v>-0.24194901688532899</v>
       </c>
+      <c r="CH6" s="21"/>
+      <c r="CI6" s="21"/>
+      <c r="CJ6" s="21"/>
+      <c r="CK6" s="21"/>
     </row>
-    <row r="7" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:89" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D7">
         <v>2000138897</v>
@@ -2944,16 +2965,16 @@
         <v>69</v>
       </c>
       <c r="I7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M7">
         <v>55</v>
@@ -3046,10 +3067,10 @@
         <v>23.79</v>
       </c>
       <c r="AQ7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AS7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AV7" s="7">
         <v>14</v>
@@ -3070,22 +3091,22 @@
         <v>2</v>
       </c>
       <c r="BC7" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD7" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="BE7" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="BF7" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="BG7" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="BF7" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="BG7" s="8" t="s">
-        <v>125</v>
-      </c>
       <c r="BH7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BN7" s="11"/>
       <c r="BP7" s="17">
@@ -3150,16 +3171,20 @@
         <f t="shared" si="6"/>
         <v>-0.77182870935289205</v>
       </c>
+      <c r="CH7" s="21"/>
+      <c r="CI7" s="21"/>
+      <c r="CJ7" s="21"/>
+      <c r="CK7" s="21"/>
     </row>
-    <row r="8" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D8">
         <v>2000148548</v>
@@ -3172,16 +3197,16 @@
         <v>90</v>
       </c>
       <c r="I8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N8">
         <v>180</v>
@@ -3271,13 +3296,13 @@
         <v>23.83</v>
       </c>
       <c r="AQ8" t="s">
+        <v>129</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS8" t="s">
         <v>130</v>
-      </c>
-      <c r="AR8" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS8" t="s">
-        <v>131</v>
       </c>
       <c r="AV8" s="7">
         <v>8</v>
@@ -3301,29 +3326,29 @@
         <v>4</v>
       </c>
       <c r="BC8" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD8" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BE8" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="BF8" s="15"/>
       <c r="BG8" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="BH8" t="s">
+        <v>99</v>
+      </c>
+      <c r="BM8" t="s">
         <v>133</v>
       </c>
-      <c r="BH8" t="s">
-        <v>100</v>
-      </c>
-      <c r="BM8" t="s">
+      <c r="BN8" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="BN8" s="11" t="s">
-        <v>135</v>
-      </c>
       <c r="BO8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="BR8" s="12">
         <v>285.32948022161196</v>
@@ -3381,16 +3406,20 @@
         <f t="shared" si="6"/>
         <v>-0.43816428159369797</v>
       </c>
+      <c r="CH8" s="21"/>
+      <c r="CI8" s="21"/>
+      <c r="CJ8" s="21"/>
+      <c r="CK8" s="21"/>
     </row>
-    <row r="9" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D9">
         <v>2001181605</v>
@@ -3409,13 +3438,13 @@
         <v>170</v>
       </c>
       <c r="I9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M9">
         <v>68</v>
@@ -3500,16 +3529,16 @@
         <v>30.84</v>
       </c>
       <c r="AQ9" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS9" t="s">
         <v>140</v>
       </c>
-      <c r="AR9" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS9" t="s">
+      <c r="AU9" t="s">
         <v>141</v>
-      </c>
-      <c r="AU9" t="s">
-        <v>142</v>
       </c>
       <c r="AV9" s="7">
         <v>15</v>
@@ -3530,29 +3559,29 @@
         <v>0</v>
       </c>
       <c r="BC9" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD9" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="BE9" s="15" t="s">
         <v>143</v>
-      </c>
-      <c r="BE9" s="15" t="s">
-        <v>144</v>
       </c>
       <c r="BF9" s="15"/>
       <c r="BG9" s="8">
         <v>42041</v>
       </c>
       <c r="BH9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="BN9" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BO9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="BP9" s="17">
         <v>19450000000</v>
@@ -3616,16 +3645,20 @@
         <f t="shared" si="6"/>
         <v>-1.1913234795044094</v>
       </c>
+      <c r="CH9" s="21"/>
+      <c r="CI9" s="21"/>
+      <c r="CJ9" s="21"/>
+      <c r="CK9" s="21"/>
     </row>
-    <row r="10" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:89" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D10">
         <v>97028369</v>
@@ -3638,10 +3671,10 @@
         <v>83</v>
       </c>
       <c r="I10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M10">
         <v>64</v>
@@ -3734,7 +3767,7 @@
         <v>19.829999999999998</v>
       </c>
       <c r="AQ10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AV10" s="7">
         <v>15</v>
@@ -3758,31 +3791,31 @@
         <v>4</v>
       </c>
       <c r="BC10" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD10" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="BE10" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="BE10" s="15" t="s">
+      <c r="BF10" s="15" t="s">
         <v>150</v>
-      </c>
-      <c r="BF10" s="15" t="s">
-        <v>151</v>
       </c>
       <c r="BG10" s="8">
         <v>42069</v>
       </c>
       <c r="BH10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="BN10" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="BO10" t="s">
         <v>88</v>
-      </c>
-      <c r="BO10" t="s">
-        <v>89</v>
       </c>
       <c r="BP10" s="17">
         <v>11175000000</v>
@@ -3846,13 +3879,17 @@
         <f t="shared" si="6"/>
         <v>-1.0092597146043005</v>
       </c>
+      <c r="CH10" s="21"/>
+      <c r="CI10" s="21"/>
+      <c r="CJ10" s="21"/>
+      <c r="CK10" s="21"/>
     </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C11">
         <v>93112314</v>
@@ -3868,13 +3905,13 @@
         <v>70</v>
       </c>
       <c r="I11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M11">
         <v>59</v>
@@ -3960,7 +3997,7 @@
         <v>10.52</v>
       </c>
       <c r="AQ11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AV11" s="7">
         <v>12</v>
@@ -3984,31 +4021,31 @@
         <v>1</v>
       </c>
       <c r="BC11" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD11" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BE11" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BF11" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BG11" s="8">
         <v>42222</v>
       </c>
       <c r="BH11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM11" t="s">
+        <v>155</v>
+      </c>
+      <c r="BN11" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="BO11" t="s">
         <v>156</v>
-      </c>
-      <c r="BN11" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="BO11" t="s">
-        <v>157</v>
       </c>
       <c r="BP11" s="17">
         <v>22725000000</v>
@@ -4072,16 +4109,20 @@
         <f t="shared" si="6"/>
         <v>-0.21214763014363278</v>
       </c>
+      <c r="CH11" s="21"/>
+      <c r="CI11" s="21"/>
+      <c r="CJ11" s="21"/>
+      <c r="CK11" s="21"/>
     </row>
-    <row r="12" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D12">
         <v>97050572</v>
@@ -4097,13 +4138,13 @@
         <v>106</v>
       </c>
       <c r="I12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M12">
         <v>72</v>
@@ -4191,7 +4232,7 @@
         <v>16.41</v>
       </c>
       <c r="AQ12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AV12" s="7">
         <v>15</v>
@@ -4209,31 +4250,31 @@
         <v>0</v>
       </c>
       <c r="BC12" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD12" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BE12" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BF12" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="BG12" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="BH12" t="s">
+        <v>99</v>
+      </c>
+      <c r="BM12" t="s">
         <v>162</v>
       </c>
-      <c r="BG12" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="BH12" t="s">
-        <v>100</v>
-      </c>
-      <c r="BM12" t="s">
-        <v>163</v>
-      </c>
       <c r="BN12" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="BO12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BP12" s="17">
         <v>35750000000</v>
@@ -4297,16 +4338,20 @@
         <f t="shared" si="6"/>
         <v>-0.34858358499125164</v>
       </c>
+      <c r="CH12" s="21"/>
+      <c r="CI12" s="21"/>
+      <c r="CJ12" s="21"/>
+      <c r="CK12" s="21"/>
     </row>
-    <row r="13" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D13">
         <v>97055803</v>
@@ -4319,13 +4364,13 @@
         <v>62</v>
       </c>
       <c r="I13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M13">
         <v>87</v>
@@ -4380,18 +4425,18 @@
         <v>3</v>
       </c>
       <c r="BC13" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BD13" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="BE13" s="15"/>
       <c r="BF13" s="15"/>
       <c r="BG13" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BH13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BP13" s="17">
         <v>18125000000</v>
@@ -4455,16 +4500,20 @@
         <f t="shared" si="6"/>
         <v>-1.7492887781108664</v>
       </c>
+      <c r="CH13" s="21"/>
+      <c r="CI13" s="21"/>
+      <c r="CJ13" s="21"/>
+      <c r="CK13" s="21"/>
     </row>
-    <row r="14" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D14">
         <v>2001183142</v>
@@ -4477,13 +4526,13 @@
         <v>77</v>
       </c>
       <c r="I14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M14">
         <v>40</v>
@@ -4564,7 +4613,7 @@
         <v>23.4</v>
       </c>
       <c r="AS14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AV14" s="7">
         <v>12</v>
@@ -4588,18 +4637,18 @@
         <v>3</v>
       </c>
       <c r="BC14" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BD14" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BE14" s="15"/>
       <c r="BF14" s="15"/>
       <c r="BG14" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="BH14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BR14" s="12"/>
       <c r="BS14" s="12"/>
@@ -4645,16 +4694,20 @@
         <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
+      <c r="CH14" s="21"/>
+      <c r="CI14" s="21"/>
+      <c r="CJ14" s="21"/>
+      <c r="CK14" s="21"/>
     </row>
-    <row r="15" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D15">
         <v>96018152</v>
@@ -4670,16 +4723,16 @@
         <v>75</v>
       </c>
       <c r="I15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M15">
         <v>70</v>
@@ -4767,7 +4820,7 @@
         <v>20.329999999999998</v>
       </c>
       <c r="AQ15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AV15" s="7">
         <v>15</v>
@@ -4791,31 +4844,31 @@
         <v>2</v>
       </c>
       <c r="BC15" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD15" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BE15" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BF15" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BG15" s="8">
         <v>42162</v>
       </c>
       <c r="BH15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BN15" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BO15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="BP15" s="17">
         <v>20150000000</v>
@@ -4873,13 +4926,17 @@
         <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
+      <c r="CH15" s="21"/>
+      <c r="CI15" s="21"/>
+      <c r="CJ15" s="21"/>
+      <c r="CK15" s="21"/>
     </row>
-    <row r="16" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:89" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D16">
         <v>97049968</v>
@@ -4892,10 +4949,10 @@
         <v>67</v>
       </c>
       <c r="I16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M16">
         <v>84</v>
@@ -4982,7 +5039,7 @@
         <v>27.77</v>
       </c>
       <c r="AQ16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AV16" s="7"/>
       <c r="AW16" s="7">
@@ -4998,40 +5055,40 @@
         <v>5</v>
       </c>
       <c r="BA16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BB16">
         <v>6</v>
       </c>
       <c r="BC16" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD16" t="s">
+        <v>178</v>
+      </c>
+      <c r="BE16" t="s">
         <v>179</v>
       </c>
-      <c r="BE16" t="s">
+      <c r="BG16" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="BG16" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="BH16" s="9" t="s">
-        <v>182</v>
+        <v>84</v>
       </c>
       <c r="BI16" s="10">
         <v>42228</v>
       </c>
       <c r="BJ16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="BM16" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="BN16" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BO16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="BP16" s="17">
         <v>8475000000</v>
@@ -5089,16 +5146,20 @@
         <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
+      <c r="CH16" s="21"/>
+      <c r="CI16" s="21"/>
+      <c r="CJ16" s="21"/>
+      <c r="CK16" s="21"/>
     </row>
-    <row r="17" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D17">
         <v>2004245733</v>
@@ -5111,13 +5172,13 @@
         <v>78</v>
       </c>
       <c r="I17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N17">
         <v>189</v>
@@ -5196,19 +5257,19 @@
         <v>22.1</v>
       </c>
       <c r="AQ17" t="s">
+        <v>183</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>184</v>
+      </c>
+      <c r="AS17" t="s">
         <v>185</v>
       </c>
-      <c r="AR17" t="s">
+      <c r="AT17" t="s">
         <v>186</v>
       </c>
-      <c r="AS17" t="s">
+      <c r="AU17" t="s">
         <v>187</v>
-      </c>
-      <c r="AT17" t="s">
-        <v>188</v>
-      </c>
-      <c r="AU17" t="s">
-        <v>189</v>
       </c>
       <c r="AV17" s="7"/>
       <c r="AW17" s="7">
@@ -5224,29 +5285,29 @@
         <v>1</v>
       </c>
       <c r="BC17" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD17" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="BE17" s="15" t="s">
         <v>126</v>
-      </c>
-      <c r="BE17" s="15" t="s">
-        <v>127</v>
       </c>
       <c r="BF17" s="15"/>
       <c r="BG17" s="8">
         <v>42192</v>
       </c>
       <c r="BH17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM17" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="BN17" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BO17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="BR17" s="12"/>
       <c r="BS17" s="12"/>
@@ -5292,13 +5353,17 @@
         <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
+      <c r="CH17" s="21"/>
+      <c r="CI17" s="21"/>
+      <c r="CJ17" s="21"/>
+      <c r="CK17" s="21"/>
     </row>
-    <row r="18" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:89" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D18">
         <v>2005285681</v>
@@ -5311,10 +5376,10 @@
         <v>71</v>
       </c>
       <c r="I18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M18">
         <v>93</v>
@@ -5396,26 +5461,26 @@
       <c r="AW18" s="7"/>
       <c r="AX18" s="7"/>
       <c r="BA18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BB18">
         <v>6</v>
       </c>
       <c r="BC18" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BD18" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="BG18" s="8"/>
       <c r="BH18" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="BI18" s="10">
         <v>42244</v>
       </c>
       <c r="BJ18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="BR18" s="12">
         <v>243.32411285861059</v>
@@ -5473,16 +5538,20 @@
         <f t="shared" si="6"/>
         <v>-0.51826148575675945</v>
       </c>
+      <c r="CH18" s="21"/>
+      <c r="CI18" s="21"/>
+      <c r="CJ18" s="21"/>
+      <c r="CK18" s="21"/>
     </row>
-    <row r="19" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D19">
         <v>991262286</v>
@@ -5498,16 +5567,16 @@
         <v>64</v>
       </c>
       <c r="I19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="L19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M19">
         <v>54</v>
@@ -5597,7 +5666,7 @@
         <v>75</v>
       </c>
       <c r="AQ19" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AV19" s="7">
         <v>15</v>
@@ -5621,16 +5690,16 @@
         <v>1</v>
       </c>
       <c r="BC19" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BD19" s="15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="BE19" s="15"/>
       <c r="BF19" s="15"/>
       <c r="BG19" s="8"/>
       <c r="BH19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BP19" s="17">
         <v>7150000000</v>
@@ -5694,16 +5763,20 @@
         <f t="shared" si="6"/>
         <v>-1.2953986744755746</v>
       </c>
+      <c r="CH19" s="21"/>
+      <c r="CI19" s="21"/>
+      <c r="CJ19" s="21"/>
+      <c r="CK19" s="21"/>
     </row>
-    <row r="20" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D20">
         <v>97056906</v>
@@ -5716,16 +5789,16 @@
         <v>57</v>
       </c>
       <c r="I20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="L20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M20">
         <v>126</v>
@@ -5818,7 +5891,7 @@
         <v>16.03</v>
       </c>
       <c r="AQ20" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AV20" s="7">
         <v>15</v>
@@ -5842,22 +5915,22 @@
         <v>3</v>
       </c>
       <c r="BC20" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BD20" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="BE20" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="BF20" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="BE20" s="15" t="s">
+      <c r="BG20" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="BF20" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="BG20" s="8" t="s">
-        <v>206</v>
-      </c>
       <c r="BH20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BP20" s="17">
         <v>21900000000</v>
@@ -5921,16 +5994,20 @@
         <f t="shared" si="6"/>
         <v>-2.9556748512361253</v>
       </c>
+      <c r="CH20" s="21"/>
+      <c r="CI20" s="21"/>
+      <c r="CJ20" s="21"/>
+      <c r="CK20" s="21"/>
     </row>
-    <row r="21" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D21">
         <v>2001178579</v>
@@ -5943,13 +6020,13 @@
         <v>72</v>
       </c>
       <c r="I21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K21" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N21">
         <v>120</v>
@@ -6036,7 +6113,7 @@
         <v>27</v>
       </c>
       <c r="AS21" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="AV21" s="7"/>
       <c r="AW21" s="7">
@@ -6058,18 +6135,18 @@
         <v>1</v>
       </c>
       <c r="BC21" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BD21" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="BE21" s="15"/>
       <c r="BF21" s="15"/>
       <c r="BG21" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="BH21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BP21" s="17">
         <v>24675000000</v>
@@ -6133,13 +6210,17 @@
         <f t="shared" si="6"/>
         <v>5.5829454405875885E-4</v>
       </c>
+      <c r="CH21" s="21"/>
+      <c r="CI21" s="21"/>
+      <c r="CJ21" s="21"/>
+      <c r="CK21" s="21"/>
     </row>
-    <row r="22" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22">
         <v>97795518</v>
@@ -6161,16 +6242,16 @@
         <v>164</v>
       </c>
       <c r="I22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K22" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M22">
         <v>69</v>
@@ -6254,16 +6335,16 @@
         <v>17.239999999999998</v>
       </c>
       <c r="AQ22" t="s">
+        <v>210</v>
+      </c>
+      <c r="AR22" t="s">
+        <v>211</v>
+      </c>
+      <c r="AS22" t="s">
         <v>212</v>
       </c>
-      <c r="AR22" t="s">
+      <c r="AU22" t="s">
         <v>213</v>
-      </c>
-      <c r="AS22" t="s">
-        <v>214</v>
-      </c>
-      <c r="AU22" t="s">
-        <v>215</v>
       </c>
       <c r="AV22" s="7">
         <v>15</v>
@@ -6287,28 +6368,28 @@
         <v>2</v>
       </c>
       <c r="BC22" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD22" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="BE22" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BF22" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="BG22" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="BH22" t="s">
+        <v>99</v>
+      </c>
+      <c r="BM22" t="s">
         <v>216</v>
       </c>
-      <c r="BG22" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="BH22" t="s">
-        <v>100</v>
-      </c>
-      <c r="BM22" t="s">
-        <v>218</v>
-      </c>
       <c r="BN22" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BR22" s="12"/>
       <c r="BS22" s="12"/>
@@ -6354,16 +6435,20 @@
         <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
+      <c r="CH22" s="21"/>
+      <c r="CI22" s="21"/>
+      <c r="CJ22" s="21"/>
+      <c r="CK22" s="21"/>
     </row>
-    <row r="23" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D23">
         <v>2000165080</v>
@@ -6375,7 +6460,7 @@
         <v>73</v>
       </c>
       <c r="I23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M23">
         <v>107</v>
@@ -6460,13 +6545,13 @@
         <v>25.47</v>
       </c>
       <c r="AQ23" t="s">
+        <v>218</v>
+      </c>
+      <c r="AR23" t="s">
+        <v>219</v>
+      </c>
+      <c r="AS23" t="s">
         <v>220</v>
-      </c>
-      <c r="AR23" t="s">
-        <v>221</v>
-      </c>
-      <c r="AS23" t="s">
-        <v>222</v>
       </c>
       <c r="AV23" s="7"/>
       <c r="AW23" s="7">
@@ -6488,31 +6573,31 @@
         <v>0</v>
       </c>
       <c r="BC23" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD23" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="BE23" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="BF23" s="15" t="s">
         <v>223</v>
-      </c>
-      <c r="BE23" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="BF23" s="15" t="s">
-        <v>225</v>
       </c>
       <c r="BG23" s="8">
         <v>42206</v>
       </c>
       <c r="BH23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM23" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="BN23" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BO23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="BR23" s="12">
         <v>36.276045575699001</v>
@@ -6570,16 +6655,20 @@
         <f t="shared" si="6"/>
         <v>-0.24983605672921785</v>
       </c>
+      <c r="CH23" s="21"/>
+      <c r="CI23" s="21"/>
+      <c r="CJ23" s="21"/>
+      <c r="CK23" s="21"/>
     </row>
-    <row r="24" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D24">
         <v>2005272962</v>
@@ -6675,10 +6764,10 @@
         <v>23.87</v>
       </c>
       <c r="AQ24" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="AR24" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="AV24" s="7">
         <v>11</v>
@@ -6694,31 +6783,31 @@
         <v>5</v>
       </c>
       <c r="BC24" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD24" s="15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="BE24" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="BF24" s="15" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="BG24" s="8">
         <v>42204</v>
       </c>
       <c r="BH24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM24" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="BN24" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BO24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="BR24" s="12">
         <v>422.79547092771963</v>
@@ -6776,16 +6865,20 @@
         <f t="shared" si="6"/>
         <v>-0.24311261824301414</v>
       </c>
+      <c r="CH24" s="21"/>
+      <c r="CI24" s="21"/>
+      <c r="CJ24" s="21"/>
+      <c r="CK24" s="21"/>
     </row>
-    <row r="25" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C25" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D25">
         <v>2000157183</v>
@@ -6887,7 +6980,7 @@
         <v>23.13</v>
       </c>
       <c r="AQ25" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AV25" s="7"/>
       <c r="AW25" s="7">
@@ -6909,18 +7002,18 @@
         <v>1</v>
       </c>
       <c r="BC25" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BD25" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="BE25" s="15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="BF25" s="15"/>
       <c r="BG25" s="8"/>
       <c r="BH25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BR25" s="12">
         <v>60.336516656107015</v>
@@ -6978,16 +7071,20 @@
         <f t="shared" si="6"/>
         <v>-1.82739440883971</v>
       </c>
+      <c r="CH25" s="21"/>
+      <c r="CI25" s="21"/>
+      <c r="CJ25" s="21"/>
+      <c r="CK25" s="21"/>
     </row>
-    <row r="26" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D26">
         <v>2002194864</v>
@@ -6999,13 +7096,13 @@
         <v>73</v>
       </c>
       <c r="I26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K26" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="N26">
         <v>163</v>
@@ -7092,10 +7189,10 @@
         <v>14.35</v>
       </c>
       <c r="AR26" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="AS26" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="AV26" s="7">
         <v>15</v>
@@ -7119,10 +7216,10 @@
         <v>0</v>
       </c>
       <c r="BC26" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BD26" s="15" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="BE26" s="15"/>
       <c r="BF26" s="15"/>
@@ -7130,7 +7227,7 @@
         <v>42215</v>
       </c>
       <c r="BH26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BP26" s="17">
         <v>414000000</v>
@@ -7194,13 +7291,17 @@
         <f t="shared" si="6"/>
         <v>-0.18391969575219608</v>
       </c>
+      <c r="CH26" s="21"/>
+      <c r="CI26" s="21"/>
+      <c r="CJ26" s="21"/>
+      <c r="CK26" s="21"/>
     </row>
-    <row r="27" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:89" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D27">
         <v>98100485</v>
@@ -7212,13 +7313,13 @@
         <v>65</v>
       </c>
       <c r="I27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K27" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="N27">
         <v>193</v>
@@ -7308,7 +7409,7 @@
         <v>32.770000000000003</v>
       </c>
       <c r="AQ27" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="AV27" s="7"/>
       <c r="AW27" s="7">
@@ -7324,33 +7425,33 @@
         <v>4</v>
       </c>
       <c r="BA27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BB27">
         <v>6</v>
       </c>
       <c r="BC27" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD27" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="BG27" s="8"/>
       <c r="BH27" s="9" t="s">
-        <v>245</v>
+        <v>84</v>
       </c>
       <c r="BI27" s="10">
         <v>42255</v>
       </c>
       <c r="BJ27" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="BM27" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="BN27" s="11"/>
       <c r="BO27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BR27" s="12"/>
       <c r="BS27" s="12"/>
@@ -7396,16 +7497,20 @@
         <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
+      <c r="CH27" s="21"/>
+      <c r="CI27" s="21"/>
+      <c r="CJ27" s="21"/>
+      <c r="CK27" s="21"/>
     </row>
-    <row r="28" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:89" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C28" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D28">
         <v>2007323731</v>
@@ -7417,13 +7522,13 @@
         <v>79</v>
       </c>
       <c r="I28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K28" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="M28">
         <v>68</v>
@@ -7513,7 +7618,7 @@
         <v>59.24</v>
       </c>
       <c r="AQ28" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AV28" s="7">
         <v>11</v>
@@ -7537,29 +7642,29 @@
         <v>5</v>
       </c>
       <c r="BC28" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD28" s="15" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="BE28" s="15" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="BF28" s="15" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="BG28" s="8"/>
       <c r="BH28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="BN28" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="BO28" t="s">
         <v>88</v>
-      </c>
-      <c r="BO28" t="s">
-        <v>89</v>
       </c>
       <c r="BR28" s="12">
         <v>100.15123801623037</v>
@@ -7617,16 +7722,20 @@
         <f t="shared" si="6"/>
         <v>-0.25473809932384112</v>
       </c>
+      <c r="CH28" s="21"/>
+      <c r="CI28" s="21"/>
+      <c r="CJ28" s="21"/>
+      <c r="CK28" s="21"/>
     </row>
-    <row r="29" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:89" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D29">
         <v>96017608</v>
@@ -7638,13 +7747,13 @@
         <v>83</v>
       </c>
       <c r="I29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K29" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="M29">
         <v>88</v>
@@ -7716,7 +7825,7 @@
         <v>13.65</v>
       </c>
       <c r="AQ29" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="AV29" s="7">
         <v>15</v>
@@ -7737,22 +7846,22 @@
         <v>0</v>
       </c>
       <c r="BB29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BC29" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BD29" s="15" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="BE29" s="15"/>
       <c r="BF29" s="15"/>
       <c r="BG29" s="8"/>
       <c r="BH29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM29" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="BR29" s="12"/>
       <c r="BS29" s="12"/>
@@ -7798,13 +7907,17 @@
         <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
+      <c r="CH29" s="21"/>
+      <c r="CI29" s="21"/>
+      <c r="CJ29" s="21"/>
+      <c r="CK29" s="21"/>
     </row>
-    <row r="30" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C30">
         <v>94835374</v>
@@ -7819,16 +7932,16 @@
         <v>82</v>
       </c>
       <c r="I30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K30" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="L30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M30">
         <v>90</v>
@@ -7915,7 +8028,7 @@
         <v>104.42</v>
       </c>
       <c r="AQ30" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="AV30" s="7">
         <v>15</v>
@@ -7930,27 +8043,27 @@
         <v>0</v>
       </c>
       <c r="BC30" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD30" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BE30" s="15" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="BF30" s="15"/>
       <c r="BG30" s="8"/>
       <c r="BH30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM30" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="BN30" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BO30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="BR30" s="12">
         <v>33.465472753958551</v>
@@ -8008,16 +8121,20 @@
         <f t="shared" si="6"/>
         <v>-0.65571937606302033</v>
       </c>
+      <c r="CH30" s="21"/>
+      <c r="CI30" s="21"/>
+      <c r="CJ30" s="21"/>
+      <c r="CK30" s="21"/>
     </row>
-    <row r="31" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D31">
         <v>97045297</v>
@@ -8026,10 +8143,10 @@
         <v>12291979</v>
       </c>
       <c r="I31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P31">
         <v>95.06</v>
@@ -8126,25 +8243,25 @@
         <v>2</v>
       </c>
       <c r="BC31" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD31" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BE31" s="15"/>
       <c r="BF31" s="15"/>
       <c r="BG31" s="8"/>
       <c r="BH31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM31" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="BN31" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BO31" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="BR31" s="12">
         <v>21.712853911108027</v>
@@ -8202,13 +8319,17 @@
         <f t="shared" si="6"/>
         <v>-2.1004283670025945</v>
       </c>
+      <c r="CH31" s="21"/>
+      <c r="CI31" s="21"/>
+      <c r="CJ31" s="21"/>
+      <c r="CK31" s="21"/>
     </row>
-    <row r="32" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:89" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D32">
         <v>2005274329</v>
@@ -8220,13 +8341,13 @@
         <v>68</v>
       </c>
       <c r="I32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K32" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="L32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M32">
         <v>67</v>
@@ -8316,7 +8437,7 @@
         <v>15.38</v>
       </c>
       <c r="AQ32" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="AV32" s="7"/>
       <c r="AW32" s="7">
@@ -8332,41 +8453,41 @@
         <v>6</v>
       </c>
       <c r="BA32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BB32">
         <v>6</v>
       </c>
       <c r="BC32" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD32" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="BE32" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="BF32" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="BG32" s="7"/>
       <c r="BH32" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="BI32" s="10">
         <v>42272</v>
       </c>
       <c r="BJ32" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="BM32" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="BN32" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BO32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="BR32" s="12">
         <v>63.81142724367502</v>
@@ -8424,13 +8545,17 @@
         <f t="shared" si="6"/>
         <v>-0.33180077573542227</v>
       </c>
+      <c r="CH32" s="21"/>
+      <c r="CI32" s="21"/>
+      <c r="CJ32" s="21"/>
+      <c r="CK32" s="21"/>
     </row>
-    <row r="33" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C33">
         <v>56638703</v>
@@ -8448,16 +8573,16 @@
         <v>73</v>
       </c>
       <c r="I33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K33" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="L33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M33">
         <v>96</v>
@@ -8547,10 +8672,10 @@
         <v>46.21</v>
       </c>
       <c r="AQ33" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="AU33" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="AV33" s="7"/>
       <c r="AW33" s="7"/>
@@ -8561,29 +8686,29 @@
         <v>0</v>
       </c>
       <c r="BC33" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD33" s="15" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="BE33" s="15" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="BF33" s="15" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="BG33" s="7"/>
       <c r="BH33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM33" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="BN33" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BO33" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="BR33" s="12"/>
       <c r="BS33" s="12"/>
@@ -8629,13 +8754,17 @@
         <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
+      <c r="CH33" s="21"/>
+      <c r="CI33" s="21"/>
+      <c r="CJ33" s="21"/>
+      <c r="CK33" s="21"/>
     </row>
-    <row r="34" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:89" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D34">
         <v>2005270050</v>
@@ -8647,7 +8776,7 @@
         <v>87</v>
       </c>
       <c r="I34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M34">
         <v>64</v>
@@ -8737,7 +8866,7 @@
         <v>30.59</v>
       </c>
       <c r="AQ34" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="AV34" s="7">
         <v>13</v>
@@ -8749,35 +8878,35 @@
         <v>5</v>
       </c>
       <c r="BA34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BB34">
         <v>6</v>
       </c>
       <c r="BC34" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD34" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="BG34" s="7"/>
       <c r="BH34" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="BI34" s="10">
         <v>42297</v>
       </c>
       <c r="BJ34" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="BM34" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="BN34" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BO34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="BR34" s="12">
         <v>62.588876636588132</v>
@@ -8835,16 +8964,20 @@
         <f t="shared" si="6"/>
         <v>-1.049687706441977</v>
       </c>
+      <c r="CH34" s="21"/>
+      <c r="CI34" s="21"/>
+      <c r="CJ34" s="21"/>
+      <c r="CK34" s="21"/>
     </row>
-    <row r="35" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>61</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D35">
         <v>2000163820</v>
@@ -8856,10 +8989,10 @@
         <v>71</v>
       </c>
       <c r="I35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M35">
         <v>100</v>
@@ -8946,7 +9079,7 @@
         <v>17.350000000000001</v>
       </c>
       <c r="AQ35" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="AV35" s="7"/>
       <c r="AW35" s="7">
@@ -8968,18 +9101,18 @@
         <v>2</v>
       </c>
       <c r="BC35" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD35" s="15" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="BE35" s="15" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="BF35" s="15"/>
       <c r="BG35" s="7"/>
       <c r="BH35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BN35" s="11"/>
       <c r="BR35" s="12">
@@ -9038,16 +9171,20 @@
         <f t="shared" si="6"/>
         <v>0.29470551948947671</v>
       </c>
+      <c r="CH35" s="21"/>
+      <c r="CI35" s="21"/>
+      <c r="CJ35" s="21"/>
+      <c r="CK35" s="21"/>
     </row>
-    <row r="36" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D36">
         <v>2000146747</v>
@@ -9059,10 +9196,10 @@
         <v>80</v>
       </c>
       <c r="I36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M36">
         <v>90</v>
@@ -9155,7 +9292,7 @@
         <v>22.37</v>
       </c>
       <c r="AQ36" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="AV36" s="7"/>
       <c r="AW36" s="7"/>
@@ -9172,27 +9309,27 @@
         <v>5</v>
       </c>
       <c r="BC36" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD36" s="15" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="BE36" s="15" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="BF36" s="15" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="BG36" s="7"/>
       <c r="BH36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM36" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="BN36" s="11"/>
       <c r="BO36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="BR36" s="12">
         <v>29.548025395890896</v>
@@ -9250,16 +9387,20 @@
         <f t="shared" si="6"/>
         <v>-0.31040434082851631</v>
       </c>
+      <c r="CH36" s="21"/>
+      <c r="CI36" s="21"/>
+      <c r="CJ36" s="21"/>
+      <c r="CK36" s="21"/>
     </row>
-    <row r="37" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>64</v>
       </c>
       <c r="B37" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C37" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D37">
         <v>2002201576</v>
@@ -9271,13 +9412,13 @@
         <v>80</v>
       </c>
       <c r="I37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K37" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="L37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M37">
         <v>81</v>
@@ -9370,13 +9511,13 @@
         <v>35.08</v>
       </c>
       <c r="AQ37" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="AS37" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="AU37" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="AV37" s="7"/>
       <c r="AW37" s="7">
@@ -9392,31 +9533,31 @@
         <v>4</v>
       </c>
       <c r="BA37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="BB37">
         <v>6</v>
       </c>
       <c r="BC37" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD37" s="15" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="BE37" s="15"/>
       <c r="BF37" s="15"/>
       <c r="BG37" s="7"/>
       <c r="BH37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM37" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="BN37" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BO37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BR37" s="12">
         <v>96.565336906632936</v>
@@ -9474,13 +9615,17 @@
         <f t="shared" si="6"/>
         <v>0.16455094925006894</v>
       </c>
+      <c r="CH37" s="21"/>
+      <c r="CI37" s="21"/>
+      <c r="CJ37" s="21"/>
+      <c r="CK37" s="21"/>
     </row>
-    <row r="38" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>66</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C38">
         <v>68202122</v>
@@ -9495,13 +9640,13 @@
         <v>38</v>
       </c>
       <c r="I38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M38">
         <v>80</v>
@@ -9576,7 +9721,7 @@
         <v>16.53</v>
       </c>
       <c r="AQ38" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="AV38" s="7">
         <v>15</v>
@@ -9600,16 +9745,16 @@
         <v>0</v>
       </c>
       <c r="BC38" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD38" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BE38" s="15"/>
       <c r="BF38" s="15"/>
       <c r="BG38" s="7"/>
       <c r="BH38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BN38" s="11"/>
       <c r="BR38" s="12">
@@ -9668,16 +9813,20 @@
         <f t="shared" si="6"/>
         <v>-0.13816872200507874</v>
       </c>
+      <c r="CH38" s="21"/>
+      <c r="CI38" s="21"/>
+      <c r="CJ38" s="21"/>
+      <c r="CK38" s="21"/>
     </row>
-    <row r="39" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>67</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C39" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D39">
         <v>98088409</v>
@@ -9695,16 +9844,16 @@
         <v>158</v>
       </c>
       <c r="I39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K39" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="L39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M39">
         <v>76</v>
@@ -9782,10 +9931,10 @@
         <v>38.28</v>
       </c>
       <c r="AQ39" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="AU39" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="AV39" s="7">
         <v>14</v>
@@ -9800,18 +9949,18 @@
         <v>5</v>
       </c>
       <c r="BC39" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BD39" s="15" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="BE39" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BF39" s="15"/>
       <c r="BG39" s="7"/>
       <c r="BH39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BR39" s="12">
         <v>40.733085976606141</v>
@@ -9869,13 +10018,17 @@
         <f t="shared" ref="CG39:CG45" si="15">(CE39/BY39)</f>
         <v>-2.18052189053906</v>
       </c>
+      <c r="CH39" s="21"/>
+      <c r="CI39" s="21"/>
+      <c r="CJ39" s="21"/>
+      <c r="CK39" s="21"/>
     </row>
-    <row r="40" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:89" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>68</v>
       </c>
       <c r="B40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C40">
         <v>82157089</v>
@@ -9887,7 +10040,7 @@
         <v>12441311</v>
       </c>
       <c r="L40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M40">
         <v>72</v>
@@ -9965,7 +10118,7 @@
         <v>24.37</v>
       </c>
       <c r="AQ40" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="AV40" s="7">
         <v>15</v>
@@ -9989,19 +10142,19 @@
         <v>0</v>
       </c>
       <c r="BC40" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD40" s="15" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="BE40" s="15"/>
       <c r="BF40" s="15"/>
       <c r="BG40" s="7"/>
       <c r="BH40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM40" s="9" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="BN40" s="11"/>
       <c r="BR40" s="12"/>
@@ -10048,16 +10201,20 @@
         <f t="shared" si="15"/>
         <v>#NUM!</v>
       </c>
+      <c r="CH40" s="21"/>
+      <c r="CI40" s="21"/>
+      <c r="CJ40" s="21"/>
+      <c r="CK40" s="21"/>
     </row>
-    <row r="41" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>71</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C41" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D41">
         <v>2007320784</v>
@@ -10072,16 +10229,16 @@
         <v>76</v>
       </c>
       <c r="I41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K41" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="L41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M41">
         <v>65</v>
@@ -10168,7 +10325,7 @@
         <v>22.28</v>
       </c>
       <c r="AQ41" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="AV41" s="7">
         <v>15</v>
@@ -10187,20 +10344,20 @@
         <v>0</v>
       </c>
       <c r="BC41" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BD41" s="15" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="BE41" s="15" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="BF41" s="15" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="BG41" s="7"/>
       <c r="BH41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BR41" s="12">
         <v>17.228219959045816</v>
@@ -10258,13 +10415,17 @@
         <f t="shared" si="15"/>
         <v>-0.76646479039948912</v>
       </c>
+      <c r="CH41" s="21"/>
+      <c r="CI41" s="21"/>
+      <c r="CJ41" s="21"/>
+      <c r="CK41" s="21"/>
     </row>
-    <row r="42" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>72</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C42">
         <v>74429292</v>
@@ -10279,13 +10440,13 @@
         <v>58</v>
       </c>
       <c r="I42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M42">
         <v>81</v>
@@ -10354,10 +10515,10 @@
         <v>21.51</v>
       </c>
       <c r="AQ42" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="AR42" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="AV42" s="7">
         <v>15</v>
@@ -10381,25 +10542,25 @@
         <v>0</v>
       </c>
       <c r="BC42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD42" s="15" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="BE42" s="15"/>
       <c r="BF42" s="15"/>
       <c r="BG42" s="7"/>
       <c r="BH42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM42" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="BN42" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BO42" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="BR42" s="12">
         <v>18.541387614315685</v>
@@ -10457,13 +10618,17 @@
         <f t="shared" si="15"/>
         <v>-0.90028416392445043</v>
       </c>
+      <c r="CH42" s="21"/>
+      <c r="CI42" s="21"/>
+      <c r="CJ42" s="21"/>
+      <c r="CK42" s="21"/>
     </row>
-    <row r="43" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>75</v>
       </c>
       <c r="B43" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C43">
         <v>82525308</v>
@@ -10481,13 +10646,13 @@
         <v>58</v>
       </c>
       <c r="I43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M43">
         <v>100</v>
@@ -10571,10 +10736,10 @@
         <v>17.8</v>
       </c>
       <c r="AQ43" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="AR43" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="AV43" s="7"/>
       <c r="AW43" s="7">
@@ -10596,29 +10761,29 @@
         <v>2</v>
       </c>
       <c r="BC43" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD43" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BE43" s="15" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="BF43" s="15" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="BG43" s="7"/>
       <c r="BH43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM43" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="BN43" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BO43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BR43" s="12">
         <v>35.886389333315194</v>
@@ -10676,16 +10841,20 @@
         <f t="shared" si="15"/>
         <v>-8.950326022742941E-2</v>
       </c>
+      <c r="CH43" s="21"/>
+      <c r="CI43" s="21"/>
+      <c r="CJ43" s="21"/>
+      <c r="CK43" s="21"/>
     </row>
-    <row r="44" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>76</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C44" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D44">
         <v>2000137300</v>
@@ -10700,16 +10869,16 @@
         <v>110</v>
       </c>
       <c r="I44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K44" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="L44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M44">
         <v>92</v>
@@ -10784,10 +10953,10 @@
         <v>32.29</v>
       </c>
       <c r="AQ44" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="AU44" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="AV44" s="7">
         <v>15</v>
@@ -10811,29 +10980,29 @@
         <v>1</v>
       </c>
       <c r="BC44" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD44" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BE44" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BF44" s="15" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="BG44" s="7"/>
       <c r="BH44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BM44" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="BN44" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BO44" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BR44" s="12">
         <v>82.685059641657787</v>
@@ -10891,16 +11060,20 @@
         <f t="shared" si="15"/>
         <v>0.13786561135993317</v>
       </c>
+      <c r="CH44" s="21"/>
+      <c r="CI44" s="21"/>
+      <c r="CJ44" s="21"/>
+      <c r="CK44" s="21"/>
     </row>
-    <row r="45" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C45" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D45">
         <v>2008345081</v>
@@ -10912,13 +11085,13 @@
         <v>69</v>
       </c>
       <c r="I45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M45">
         <v>64</v>
@@ -11011,7 +11184,7 @@
         <v>12.19</v>
       </c>
       <c r="AQ45" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="AV45" s="7">
         <v>14</v>
@@ -11021,20 +11194,20 @@
         <v>1</v>
       </c>
       <c r="BC45" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BD45" s="15" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="BE45" s="15" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="BF45" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BG45" s="7"/>
       <c r="BH45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BR45" s="12"/>
       <c r="BS45" s="12"/>
@@ -11080,6 +11253,10 @@
         <f t="shared" si="15"/>
         <v>#NUM!</v>
       </c>
+      <c r="CH45" s="21"/>
+      <c r="CI45" s="21"/>
+      <c r="CJ45" s="21"/>
+      <c r="CK45" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>